<commit_message>
Añadido código AVX con vectorización manual mediante intrínsecos
</commit_message>
<xml_diff>
--- a/practicas/practica1/resultados.xlsx
+++ b/practicas/practica1/resultados.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbarelop/src/unizar/MP-1617/practicas/practica1/resultados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbarelop/src/unizar/MP-1617/practicas/practica1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="4140" windowWidth="35740" windowHeight="17120" tabRatio="500"/>
+    <workbookView xWindow="55420" yWindow="2360" windowWidth="20520" windowHeight="18900" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="i5-4570 (lab102-194)" sheetId="2" r:id="rId1"/>
+    <sheet name="i5-4570 (lab004-071)" sheetId="2" r:id="rId1"/>
     <sheet name="i5-3470" sheetId="1" r:id="rId2"/>
     <sheet name="i7-4770" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="24">
   <si>
     <t>Versión</t>
   </si>
@@ -161,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -198,35 +198,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -235,6 +213,122 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -242,12 +336,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,16 +359,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -285,11 +387,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,7 +700,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,34 +709,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="8" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
@@ -612,65 +744,65 @@
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
+      <c r="V1" s="13"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -684,16 +816,16 @@
       <c r="C3" s="2">
         <v>2000</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="16">
         <v>5.01</v>
       </c>
       <c r="F3" s="2">
-        <v>500.9</v>
-      </c>
-      <c r="G3" s="6">
+        <v>500.8</v>
+      </c>
+      <c r="G3" s="5">
         <v>1.2</v>
       </c>
       <c r="H3" s="2">
@@ -703,11 +835,11 @@
         <f>$E$3/E3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="17">
         <f>2/E3</f>
         <v>0.39920159680638723</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="16">
         <v>1.28</v>
       </c>
       <c r="L3" s="2">
@@ -723,29 +855,29 @@
         <f>$K$3/K3</f>
         <v>1</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="17">
         <f>2/M3</f>
         <v>0.4081632653061224</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="13" t="e">
+      <c r="Q3" s="16">
+        <v>0.76</v>
+      </c>
+      <c r="R3" s="2">
+        <v>76</v>
+      </c>
+      <c r="S3" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="T3" s="3">
+        <v>956991104</v>
+      </c>
+      <c r="U3" s="7">
         <f>$Q$3/Q3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V3" s="13" t="e">
+        <v>1</v>
+      </c>
+      <c r="V3" s="21">
         <f>2/S3</f>
-        <v>#VALUE!</v>
+        <v>0.24390243902439027</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -758,16 +890,16 @@
       <c r="C4" s="2">
         <v>2000</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.77</v>
+      <c r="E4" s="16">
+        <v>0.76</v>
       </c>
       <c r="F4" s="2">
-        <v>76.8</v>
-      </c>
-      <c r="G4" s="6">
+        <v>77.5</v>
+      </c>
+      <c r="G4" s="5">
         <v>8.1</v>
       </c>
       <c r="H4" s="2">
@@ -775,13 +907,13 @@
       </c>
       <c r="I4" s="2">
         <f>$E$3/E4</f>
-        <v>6.5064935064935057</v>
-      </c>
-      <c r="J4" s="2">
+        <v>6.5921052631578947</v>
+      </c>
+      <c r="J4" s="17">
         <f>2/E4</f>
-        <v>2.5974025974025974</v>
-      </c>
-      <c r="K4" s="2">
+        <v>2.6315789473684212</v>
+      </c>
+      <c r="K4" s="16">
         <v>1.28</v>
       </c>
       <c r="L4" s="2">
@@ -794,32 +926,32 @@
         <v>956991104</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" ref="O4:O7" si="0">$K$3/K4</f>
+        <f t="shared" ref="O4:O5" si="0">$K$3/K4</f>
         <v>1</v>
       </c>
-      <c r="P4" s="2">
-        <f t="shared" ref="P4:P7" si="1">2/M4</f>
+      <c r="P4" s="17">
+        <f t="shared" ref="P4:P5" si="1">2/M4</f>
         <v>0.4081632653061224</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U4" s="13" t="e">
-        <f t="shared" ref="U4:U7" si="2">$Q$3/Q4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V4" s="13" t="e">
-        <f t="shared" ref="V4:V7" si="3">2/S4</f>
-        <v>#VALUE!</v>
+      <c r="Q4" s="16">
+        <v>0.76</v>
+      </c>
+      <c r="R4" s="2">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="S4" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="T4" s="3">
+        <v>956991104</v>
+      </c>
+      <c r="U4" s="7">
+        <f>$Q$3/Q4</f>
+        <v>1</v>
+      </c>
+      <c r="V4" s="21">
+        <f t="shared" ref="V4:V5" si="2">2/S4</f>
+        <v>0.24390243902439027</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -832,16 +964,16 @@
       <c r="C5" s="2">
         <v>2000</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="16">
         <v>0.65</v>
       </c>
       <c r="F5" s="2">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="G5" s="6">
+        <v>64.8</v>
+      </c>
+      <c r="G5" s="5">
         <v>9.6999999999999993</v>
       </c>
       <c r="H5" s="2">
@@ -851,15 +983,15 @@
         <f>$E$3/E5</f>
         <v>7.707692307692307</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" ref="J5:J8" si="4">2/E5</f>
+      <c r="J5" s="17">
+        <f t="shared" ref="J5" si="3">2/E5</f>
         <v>3.0769230769230766</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="16">
         <v>1.2</v>
       </c>
       <c r="L5" s="2">
-        <v>120.2</v>
+        <v>120.3</v>
       </c>
       <c r="M5" s="2">
         <v>5.2</v>
@@ -871,29 +1003,29 @@
         <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="17">
         <f t="shared" si="1"/>
         <v>0.38461538461538458</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U5" s="13" t="e">
+      <c r="Q5" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="R5" s="2">
+        <v>64.7</v>
+      </c>
+      <c r="S5" s="2">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="T5" s="2">
+        <v>956991104</v>
+      </c>
+      <c r="U5" s="7">
+        <f t="shared" ref="U4:U5" si="4">$Q$3/Q5</f>
+        <v>1.1692307692307693</v>
+      </c>
+      <c r="V5" s="21">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V5" s="13" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>0.2061855670103093</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -906,10 +1038,10 @@
       <c r="C6" s="2">
         <v>2000</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -925,11 +1057,11 @@
         <f>$E$3/E6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J6" s="2" t="e">
+      <c r="J6" s="17" t="e">
         <f>2/E6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="16" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -945,11 +1077,11 @@
         <f>$K$3/K6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P6" s="2" t="e">
+      <c r="P6" s="17" t="e">
         <f>2/M6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="16" t="s">
         <v>17</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -961,16 +1093,16 @@
       <c r="T6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U6" s="13" t="e">
+      <c r="U6" s="7" t="e">
         <f>$Q$3/Q6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="V6" s="13" t="e">
+      <c r="V6" s="21" t="e">
         <f>2/S6</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -980,79 +1112,79 @@
       <c r="C7" s="2">
         <v>2000</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="e">
+      <c r="E7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="19" t="e">
         <f>$E$3/E7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" s="2" t="e">
+      <c r="J7" s="20" t="e">
         <f>2/E7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="2" t="e">
+      <c r="K7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="19" t="e">
         <f>$K$3/K7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P7" s="2" t="e">
+      <c r="P7" s="20" t="e">
         <f>2/M7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U7" s="13" t="e">
+      <c r="Q7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="22" t="e">
         <f>$Q$3/Q7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="V7" s="13" t="e">
+      <c r="V7" s="23" t="e">
         <f>2/S7</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="K1:P1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:J1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="K1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1074,42 +1206,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1675,42 +1807,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1899,7 @@
       <c r="F3" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>8.9</v>
       </c>
       <c r="H3" s="2">
@@ -1817,7 +1949,7 @@
       <c r="F4" s="2">
         <v>57.4</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>10.3</v>
       </c>
       <c r="H4" s="2">
@@ -1867,7 +1999,7 @@
       <c r="F5" s="2">
         <v>511.5</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>1.2</v>
       </c>
       <c r="H5" s="2">

</xml_diff>

<commit_message>
Añadido análisis para vectores de doble precisión
</commit_message>
<xml_diff>
--- a/practicas/practica1/resultados.xlsx
+++ b/practicas/practica1/resultados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="55420" yWindow="2360" windowWidth="20520" windowHeight="18900" tabRatio="500"/>
+    <workbookView xWindow="11940" yWindow="3380" windowWidth="13660" windowHeight="12200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i5-4570 (lab004-071)" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="25">
   <si>
     <t>Versión</t>
   </si>
@@ -102,11 +102,17 @@
   <si>
     <t>GFLOPS</t>
   </si>
+  <si>
+    <t>Double</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -161,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -198,118 +204,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -335,8 +229,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -344,8 +376,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -362,23 +396,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,13 +420,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,26 +435,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -697,181 +753,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="11"/>
+    <col min="10" max="10" width="11.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="16" width="10.83203125" style="11"/>
+    <col min="17" max="20" width="10.83203125" style="1"/>
+    <col min="21" max="22" width="10.83203125" style="11"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="13"/>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
       <c r="P1" s="13"/>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
       <c r="V1" s="13"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="14" t="s">
+    <row r="2" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="16">
         <v>2000</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="18">
         <v>5.01</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="16">
         <v>500.8</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="19">
         <v>1.2</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="16">
         <v>956991104</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="20">
         <f>$E$3/E3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="21">
         <f>2/E3</f>
         <v>0.39920159680638723</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="18">
         <v>1.28</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="16">
         <v>128.30000000000001</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="16">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="16">
         <v>956991104</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="20">
         <f>$K$3/K3</f>
         <v>1</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="21">
         <f>2/M3</f>
         <v>0.4081632653061224</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="18">
         <v>0.76</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="16">
         <v>76</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="16">
         <v>8.1999999999999993</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="22">
         <v>956991104</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="20">
         <f>$Q$3/Q3</f>
         <v>1</v>
       </c>
@@ -890,10 +953,10 @@
       <c r="C4" s="2">
         <v>2000</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="14">
         <v>0.76</v>
       </c>
       <c r="F4" s="2">
@@ -905,15 +968,15 @@
       <c r="H4" s="2">
         <v>956991104</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="10">
         <f>$E$3/E4</f>
         <v>6.5921052631578947</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="15">
         <f>2/E4</f>
         <v>2.6315789473684212</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="14">
         <v>1.28</v>
       </c>
       <c r="L4" s="2">
@@ -925,15 +988,15 @@
       <c r="N4" s="2">
         <v>956991104</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="10">
         <f t="shared" ref="O4:O5" si="0">$K$3/K4</f>
         <v>1</v>
       </c>
-      <c r="P4" s="17">
+      <c r="P4" s="15">
         <f t="shared" ref="P4:P5" si="1">2/M4</f>
         <v>0.4081632653061224</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="14">
         <v>0.76</v>
       </c>
       <c r="R4" s="2">
@@ -945,11 +1008,11 @@
       <c r="T4" s="3">
         <v>956991104</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="10">
         <f>$Q$3/Q4</f>
         <v>1</v>
       </c>
-      <c r="V4" s="21">
+      <c r="V4" s="15">
         <f t="shared" ref="V4:V5" si="2">2/S4</f>
         <v>0.24390243902439027</v>
       </c>
@@ -964,10 +1027,10 @@
       <c r="C5" s="2">
         <v>2000</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="14">
         <v>0.65</v>
       </c>
       <c r="F5" s="2">
@@ -979,15 +1042,15 @@
       <c r="H5" s="2">
         <v>956991104</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="10">
         <f>$E$3/E5</f>
         <v>7.707692307692307</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
         <f t="shared" ref="J5" si="3">2/E5</f>
         <v>3.0769230769230766</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="14">
         <v>1.2</v>
       </c>
       <c r="L5" s="2">
@@ -999,15 +1062,15 @@
       <c r="N5" s="2">
         <v>956991104</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="10">
         <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
-      <c r="P5" s="17">
+      <c r="P5" s="15">
         <f t="shared" si="1"/>
         <v>0.38461538461538458</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="14">
         <v>0.65</v>
       </c>
       <c r="R5" s="2">
@@ -1019,11 +1082,11 @@
       <c r="T5" s="2">
         <v>956991104</v>
       </c>
-      <c r="U5" s="7">
-        <f t="shared" ref="U4:U5" si="4">$Q$3/Q5</f>
+      <c r="U5" s="10">
+        <f t="shared" ref="U5" si="4">$Q$3/Q5</f>
         <v>1.1692307692307693</v>
       </c>
-      <c r="V5" s="21">
+      <c r="V5" s="15">
         <f t="shared" si="2"/>
         <v>0.2061855670103093</v>
       </c>
@@ -1038,10 +1101,10 @@
       <c r="C6" s="2">
         <v>2000</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1053,15 +1116,15 @@
       <c r="H6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="2" t="e">
+      <c r="I6" s="10" t="e">
         <f>$E$3/E6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J6" s="17" t="e">
+      <c r="J6" s="15" t="e">
         <f>2/E6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1073,15 +1136,15 @@
       <c r="N6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="2" t="e">
+      <c r="O6" s="10" t="e">
         <f>$K$3/K6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P6" s="17" t="e">
+      <c r="P6" s="15" t="e">
         <f>2/M6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="Q6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -1093,16 +1156,16 @@
       <c r="T6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U6" s="7" t="e">
+      <c r="U6" s="10" t="e">
         <f>$Q$3/Q6</f>
         <v>#VALUE!</v>
       </c>
-      <c r="V6" s="21" t="e">
+      <c r="V6" s="15" t="e">
         <f>2/S6</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1112,67 +1175,437 @@
       <c r="C7" s="2">
         <v>2000</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="19" t="e">
+      <c r="E7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="10" t="e">
         <f>$E$3/E7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" s="20" t="e">
+      <c r="J7" s="15" t="e">
         <f>2/E7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="19" t="e">
+      <c r="K7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="10" t="e">
         <f>$K$3/K7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P7" s="20" t="e">
+      <c r="P7" s="15" t="e">
         <f>2/M7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="U7" s="22" t="e">
+      <c r="Q7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="10" t="e">
         <f>$Q$3/Q7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="V7" s="23" t="e">
+      <c r="V7" s="15" t="e">
         <f>2/S7</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14">
+        <v>5.08</v>
+      </c>
+      <c r="F8" s="2">
+        <v>508.3</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>999999905</v>
+      </c>
+      <c r="I8" s="10">
+        <f>$E$8/E8</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="15">
+        <f>2/E8</f>
+        <v>0.39370078740157477</v>
+      </c>
+      <c r="K8" s="14">
+        <v>2.57</v>
+      </c>
+      <c r="L8" s="2">
+        <v>257.5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>999999905</v>
+      </c>
+      <c r="O8" s="10">
+        <f>$K$8/K8</f>
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
+        <f>2/M8</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="R8" s="2">
+        <v>149.6</v>
+      </c>
+      <c r="S8" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="T8" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="U8" s="10">
+        <f>$Q$8/Q8</f>
+        <v>1</v>
+      </c>
+      <c r="V8" s="15">
+        <f>2/S8</f>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="G9" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" ref="I9:I12" si="5">$E$8/E9</f>
+        <v>3.3866666666666667</v>
+      </c>
+      <c r="J9" s="15">
+        <f>2/E9</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="K9" s="14">
+        <v>2.58</v>
+      </c>
+      <c r="L9" s="2">
+        <v>258.3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="N9" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="O9" s="10">
+        <f t="shared" ref="O9:O12" si="6">$K$8/K9</f>
+        <v>0.99612403100775182</v>
+      </c>
+      <c r="P9" s="15">
+        <f t="shared" ref="P9:P10" si="7">2/M9</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="R9" s="2">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="S9" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="T9" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="U9" s="10">
+        <f t="shared" ref="U9:U12" si="8">$Q$8/Q9</f>
+        <v>1</v>
+      </c>
+      <c r="V9" s="15">
+        <f t="shared" ref="V9:V10" si="9">2/S9</f>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>124.7</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>999999905</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="5"/>
+        <v>4.0640000000000001</v>
+      </c>
+      <c r="J10" s="15">
+        <f t="shared" ref="J10" si="10">2/E10</f>
+        <v>1.6</v>
+      </c>
+      <c r="K10" s="14">
+        <v>2.39</v>
+      </c>
+      <c r="L10" s="2">
+        <v>238.9</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="N10" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="O10" s="10">
+        <f t="shared" si="6"/>
+        <v>1.0753138075313806</v>
+      </c>
+      <c r="P10" s="15">
+        <f t="shared" si="7"/>
+        <v>0.76923076923076916</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="R10" s="2">
+        <v>124.6</v>
+      </c>
+      <c r="S10" s="2">
+        <v>5</v>
+      </c>
+      <c r="T10" s="3">
+        <v>999999905</v>
+      </c>
+      <c r="U10" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2</v>
+      </c>
+      <c r="V10" s="15">
+        <f t="shared" si="9"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J11" s="15" t="e">
+        <f>2/E11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="10" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="15" t="e">
+        <f>2/M11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" s="10" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V11" s="15" t="e">
+        <f>2/S11</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J12" s="15" t="e">
+        <f>2/E12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="10" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="15" t="e">
+        <f>2/M12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U12" s="10" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V12" s="15" t="e">
+        <f>2/S12</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1206,42 +1639,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1807,42 +2240,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>